<commit_message>
Set Docx 18 March
</commit_message>
<xml_diff>
--- a/py/Direcc.xlsx
+++ b/py/Direcc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thebr\OneDrive\Escritorio\Trabajo Gobierno\Febrero\HORUS\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7522F93-9E58-424E-8C97-B229740C3234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D3C01B-445B-49C4-A70E-DF218937890A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A414B5A2-60C7-4F45-8BD6-994228E878CD}"/>
   </bookViews>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EC664C-F74D-48DB-B806-F62A56262156}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1333,6 +1333,18 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D27">
     <sortCondition descending="1" ref="D27"/>
   </sortState>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Move Graph Defensoria DDHH -> Legal
</commit_message>
<xml_diff>
--- a/py/Direcc.xlsx
+++ b/py/Direcc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thebr\OneDrive\Escritorio\Trabajo Gobierno\Febrero\HORUS\py\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XAMPP\htdocs\HORUS\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DD8EF5-BD3E-485F-9568-2A84F9A360DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3AE9C7-C193-4B2D-B359-28FE42F2718C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A414B5A2-60C7-4F45-8BD6-994228E878CD}"/>
   </bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,6 +587,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1">
+        <f>D29</f>
+        <v>403</v>
+      </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
@@ -599,25 +603,26 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D28" si="0">SUM(B2:C2)</f>
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E2">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F2">
         <f>(B2/E2)</f>
-        <v>0.23224043715846995</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="G2">
         <f>(F2)*100</f>
-        <v>23.224043715846996</v>
+        <v>23.076923076923077</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -625,25 +630,26 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F28" si="1">(B3/E3)</f>
-        <v>5.1912568306010931E-2</v>
+        <v>4.9627791563275438E-2</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G28" si="2">(F3)*100</f>
-        <v>5.1912568306010929</v>
+        <v>4.9627791563275441</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -651,25 +657,26 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E4">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>5.1912568306010931E-2</v>
+        <v>4.9627791563275438E-2</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>5.1912568306010929</v>
+        <v>4.9627791563275441</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -687,15 +694,16 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>8.1967213114754103E-3</v>
+        <v>7.4441687344913151E-3</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>0.81967213114754101</v>
+        <v>0.74441687344913154</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -703,25 +711,26 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>2.4590163934426229E-2</v>
+        <v>2.4813895781637719E-2</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>2.459016393442623</v>
+        <v>2.481389578163772</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -729,25 +738,26 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E7">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>2.7322404371584699E-3</v>
+        <v>1.488833746898263E-2</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>0.27322404371584702</v>
+        <v>1.4888337468982631</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -755,25 +765,26 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>13</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E8">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>9.5628415300546443E-2</v>
+        <v>9.9255583126550875E-2</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>9.5628415300546443</v>
+        <v>9.9255583126550881</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -781,25 +792,26 @@
         <v>23</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E9">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>4.3715846994535519E-2</v>
+        <v>4.7146401985111663E-2</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>4.3715846994535523</v>
+        <v>4.7146401985111659</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -817,15 +829,16 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>1.912568306010929E-2</v>
+        <v>1.7369727047146403E-2</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>1.9125683060109291</v>
+        <v>1.7369727047146404</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -843,15 +856,16 @@
         <v>29</v>
       </c>
       <c r="E11">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>6.2841530054644809E-2</v>
+        <v>5.7071960297766747E-2</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>6.2841530054644812</v>
+        <v>5.7071960297766751</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -859,25 +873,26 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E12">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>5.4644808743169397E-2</v>
+        <v>5.4590570719602979E-2</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>5.4644808743169397</v>
+        <v>5.4590570719602978</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -888,22 +903,23 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>4.0983606557377046E-2</v>
+        <v>3.7220843672456573E-2</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>4.0983606557377046</v>
+        <v>3.7220843672456572</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -911,25 +927,26 @@
         <v>27</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>2.185792349726776E-2</v>
+        <v>2.2332506203473945E-2</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>2.1857923497267762</v>
+        <v>2.2332506203473943</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -937,25 +954,26 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E15">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>8.1967213114754103E-3</v>
+        <v>9.9255583126550868E-3</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>0.81967213114754101</v>
+        <v>0.99255583126550873</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -963,25 +981,26 @@
         <v>28</v>
       </c>
       <c r="B16">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E16">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>6.0109289617486336E-2</v>
+        <v>6.4516129032258063E-2</v>
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>6.0109289617486334</v>
+        <v>6.4516129032258061</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -989,25 +1008,26 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="E17">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>3.825136612021858E-2</v>
+        <v>3.7220843672456573E-2</v>
       </c>
       <c r="G17">
         <f t="shared" si="2"/>
-        <v>3.8251366120218582</v>
+        <v>3.7220843672456572</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1015,25 +1035,26 @@
         <v>12</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E18">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>1.3661202185792349E-2</v>
+        <v>1.488833746898263E-2</v>
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>1.3661202185792349</v>
+        <v>1.4888337468982631</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1044,22 +1065,23 @@
         <v>13</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>3.5519125683060107E-2</v>
+        <v>3.2258064516129031E-2</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>3.5519125683060109</v>
+        <v>3.225806451612903</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1077,15 +1099,16 @@
         <v>10</v>
       </c>
       <c r="E20">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>2.7322404371584699E-2</v>
+        <v>2.4813895781637719E-2</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>2.7322404371584699</v>
+        <v>2.481389578163772</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1103,15 +1126,16 @@
         <v>2</v>
       </c>
       <c r="E21">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>5.4644808743169399E-3</v>
+        <v>4.9627791563275434E-3</v>
       </c>
       <c r="G21">
         <f t="shared" si="2"/>
-        <v>0.54644808743169404</v>
+        <v>0.49627791563275436</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1129,15 +1153,16 @@
         <v>4</v>
       </c>
       <c r="E22">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>1.092896174863388E-2</v>
+        <v>9.9255583126550868E-3</v>
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>1.0928961748633881</v>
+        <v>0.99255583126550873</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1155,15 +1180,16 @@
         <v>2</v>
       </c>
       <c r="E23">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>5.4644808743169399E-3</v>
+        <v>4.9627791563275434E-3</v>
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>0.54644808743169404</v>
+        <v>0.49627791563275436</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1171,25 +1197,26 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E24">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>4.6448087431693992E-2</v>
+        <v>4.7146401985111663E-2</v>
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>4.6448087431693992</v>
+        <v>4.7146401985111659</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1200,22 +1227,23 @@
         <v>4</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>1.092896174863388E-2</v>
+        <v>9.9255583126550868E-3</v>
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>1.0928961748633881</v>
+        <v>0.99255583126550873</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1233,15 +1261,16 @@
         <v>3</v>
       </c>
       <c r="E26">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>8.1967213114754103E-3</v>
+        <v>7.4441687344913151E-3</v>
       </c>
       <c r="G26">
         <f t="shared" si="2"/>
-        <v>0.81967213114754101</v>
+        <v>0.74441687344913154</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1252,22 +1281,23 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>1.6393442622950821E-2</v>
+        <v>1.488833746898263E-2</v>
       </c>
       <c r="G27">
         <f t="shared" si="2"/>
-        <v>1.639344262295082</v>
+        <v>1.4888337468982631</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1275,25 +1305,26 @@
         <v>35</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E28">
-        <v>366</v>
+        <f>D29</f>
+        <v>403</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>2.7322404371584699E-3</v>
+        <v>4.9627791563275434E-3</v>
       </c>
       <c r="G28">
         <f t="shared" si="2"/>
-        <v>0.27322404371584702</v>
+        <v>0.49627791563275436</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1302,14 +1333,14 @@
       </c>
       <c r="D29">
         <f>SUM(B2:B28)</f>
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
       </c>
       <c r="F29">
         <f>SUM(F2:F28)</f>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <f>SUM(G2:G28)</f>
@@ -1322,7 +1353,7 @@
       </c>
       <c r="D30">
         <f>MEDIAN(D2:D27)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1347,6 +1378,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9d79ead9-ccf6-4ca1-bf50-acff66080910" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100747A2AC1B2A2EC4D9777D92AB3C1606A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="09a69fa5213838aa2509153927f32dac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9d79ead9-ccf6-4ca1-bf50-acff66080910" xmlns:ns4="570fb897-d274-4457-aa38-b13802a1744e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5f278dbff8306a56c26a3beb38da730" ns3:_="" ns4:_="">
     <xsd:import namespace="9d79ead9-ccf6-4ca1-bf50-acff66080910"/>
@@ -1573,24 +1621,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{534DA14E-2438-488D-BCE6-7785D8723E22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9d79ead9-ccf6-4ca1-bf50-acff66080910"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="570fb897-d274-4457-aa38-b13802a1744e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9d79ead9-ccf6-4ca1-bf50-acff66080910" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8087EB69-BA50-4370-90EF-9370E79F5015}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61C0F8AD-02DC-494A-81E4-AE7B61AFE288}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1607,29 +1663,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8087EB69-BA50-4370-90EF-9370E79F5015}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{534DA14E-2438-488D-BCE6-7785D8723E22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9d79ead9-ccf6-4ca1-bf50-acff66080910"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="570fb897-d274-4457-aa38-b13802a1744e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Set rendimientos 13 May
</commit_message>
<xml_diff>
--- a/py/Direcc.xlsx
+++ b/py/Direcc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XAMPP\htdocs\HORUS\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBD56F7-8B11-4326-B750-45F3B1A3BF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D8BBBB-E67D-4047-9073-5B3563D6D4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A414B5A2-60C7-4F45-8BD6-994228E878CD}"/>
   </bookViews>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EC664C-F74D-48DB-B806-F62A56262156}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,7 +589,7 @@
       </c>
       <c r="E1">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -603,26 +603,26 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D28" si="0">SUM(B2:C2)</f>
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="E2">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F2">
         <f>(B2/E2)</f>
-        <v>0.22317596566523606</v>
+        <v>0.22264875239923224</v>
       </c>
       <c r="G2">
         <f>(F2)*100</f>
-        <v>22.317596566523605</v>
+        <v>22.264875239923224</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -630,26 +630,26 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F28" si="1">(B3/E3)</f>
-        <v>6.0085836909871244E-2</v>
+        <v>5.5662188099808059E-2</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G28" si="2">(F3)*100</f>
-        <v>6.0085836909871242</v>
+        <v>5.5662188099808061</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -657,26 +657,26 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E4">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>6.2231759656652362E-2</v>
+        <v>7.8694817658349334E-2</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>6.2231759656652361</v>
+        <v>7.8694817658349336</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -695,15 +695,15 @@
       </c>
       <c r="E5">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>1.0729613733905579E-2</v>
+        <v>9.5969289827255271E-3</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>1.0729613733905579</v>
+        <v>0.95969289827255266</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -711,10 +711,10 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -722,15 +722,15 @@
       </c>
       <c r="E6">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>2.575107296137339E-2</v>
+        <v>2.6871401151631478E-2</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>2.5751072961373391</v>
+        <v>2.6871401151631478</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -741,23 +741,23 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>1.2875536480686695E-2</v>
+        <v>1.1516314779270634E-2</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>1.2875536480686696</v>
+        <v>1.1516314779270633</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -765,26 +765,26 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E8">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>8.7982832618025753E-2</v>
+        <v>9.2130518234165071E-2</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>8.7982832618025757</v>
+        <v>9.2130518234165066</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -792,26 +792,26 @@
         <v>23</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>4.07725321888412E-2</v>
+        <v>4.0307101727447218E-2</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>4.0772532188841204</v>
+        <v>4.0307101727447217</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -830,15 +830,15 @@
       </c>
       <c r="E10">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>1.7167381974248927E-2</v>
+        <v>1.5355086372360844E-2</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>1.7167381974248928</v>
+        <v>1.5355086372360844</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -849,23 +849,23 @@
         <v>23</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>4.9356223175965663E-2</v>
+        <v>4.4145873320537425E-2</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>4.9356223175965663</v>
+        <v>4.4145873320537428</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -873,26 +873,26 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>5.1502145922746781E-2</v>
+        <v>4.9904030710172742E-2</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>5.1502145922746783</v>
+        <v>4.9904030710172744</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -903,23 +903,23 @@
         <v>17</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>3.6480686695278972E-2</v>
+        <v>3.2629558541266791E-2</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>3.648068669527897</v>
+        <v>3.262955854126679</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -938,15 +938,15 @@
       </c>
       <c r="E14">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>2.1459227467811159E-2</v>
+        <v>1.9193857965451054E-2</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>2.1459227467811157</v>
+        <v>1.9193857965451053</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -965,15 +965,15 @@
       </c>
       <c r="E15">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>1.0729613733905579E-2</v>
+        <v>9.5969289827255271E-3</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>1.0729613733905579</v>
+        <v>0.95969289827255266</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -981,26 +981,26 @@
         <v>28</v>
       </c>
       <c r="B16">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16">
         <v>10</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E16">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>7.2961373390557943E-2</v>
+        <v>6.71785028790787E-2</v>
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>7.296137339055794</v>
+        <v>6.7178502879078703</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1008,26 +1008,26 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E17">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>3.6480686695278972E-2</v>
+        <v>4.0307101727447218E-2</v>
       </c>
       <c r="G17">
         <f t="shared" si="2"/>
-        <v>3.648068669527897</v>
+        <v>4.0307101727447217</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1035,26 +1035,26 @@
         <v>12</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>1.5021459227467811E-2</v>
+        <v>1.7274472168905951E-2</v>
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>1.502145922746781</v>
+        <v>1.727447216890595</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1062,26 +1062,26 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E19">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>3.2188841201716736E-2</v>
+        <v>3.4548944337811902E-2</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>3.2188841201716736</v>
+        <v>3.45489443378119</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1100,15 +1100,15 @@
       </c>
       <c r="E20">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>2.3605150214592276E-2</v>
+        <v>2.1113243761996161E-2</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>2.3605150214592276</v>
+        <v>2.1113243761996161</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1127,15 +1127,15 @@
       </c>
       <c r="E21">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
-        <v>6.4377682403433476E-3</v>
+        <v>5.7581573896353169E-3</v>
       </c>
       <c r="G21">
         <f t="shared" si="2"/>
-        <v>0.64377682403433478</v>
+        <v>0.57581573896353166</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1154,15 +1154,15 @@
       </c>
       <c r="E22">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>1.0729613733905579E-2</v>
+        <v>9.5969289827255271E-3</v>
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>1.0729613733905579</v>
+        <v>0.95969289827255266</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1181,15 +1181,15 @@
       </c>
       <c r="E23">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>6.4377682403433476E-3</v>
+        <v>5.7581573896353169E-3</v>
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>0.64377682403433478</v>
+        <v>0.57581573896353166</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1208,15 +1208,15 @@
       </c>
       <c r="E24">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>4.5064377682403435E-2</v>
+        <v>4.0307101727447218E-2</v>
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>4.5064377682403434</v>
+        <v>4.0307101727447217</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1224,26 +1224,26 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E25">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>1.0729613733905579E-2</v>
+        <v>1.1516314779270634E-2</v>
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>1.0729613733905579</v>
+        <v>1.1516314779270633</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1262,15 +1262,15 @@
       </c>
       <c r="E26">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>8.5836909871244635E-3</v>
+        <v>7.677543186180422E-3</v>
       </c>
       <c r="G26">
         <f t="shared" si="2"/>
-        <v>0.85836909871244638</v>
+        <v>0.76775431861804222</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1278,26 +1278,26 @@
         <v>34</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F27">
         <f t="shared" si="1"/>
-        <v>1.5021459227467811E-2</v>
+        <v>1.5355086372360844E-2</v>
       </c>
       <c r="G27">
         <f t="shared" si="2"/>
-        <v>1.502145922746781</v>
+        <v>1.5355086372360844</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1305,26 +1305,26 @@
         <v>35</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E28">
         <f>D29</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>6.4377682403433476E-3</v>
+        <v>1.5355086372360844E-2</v>
       </c>
       <c r="G28">
         <f t="shared" si="2"/>
-        <v>0.64377682403433478</v>
+        <v>1.5355086372360844</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1333,14 +1333,14 @@
       </c>
       <c r="D29">
         <f>SUM(B2:B28)</f>
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
       </c>
       <c r="F29">
         <f>SUM(F2:F28)</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="G29">
         <f>SUM(G2:G28)</f>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="D30">
         <f>MEDIAN(D2:D27)</f>
-        <v>14.5</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Scrpt and Update rendimintos 19 - Mayo
</commit_message>
<xml_diff>
--- a/py/Direcc.xlsx
+++ b/py/Direcc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XAMPP\htdocs\HORUS\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D8BBBB-E67D-4047-9073-5B3563D6D4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7932667D-FC47-4BE4-83BB-C89088B4E70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A414B5A2-60C7-4F45-8BD6-994228E878CD}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>Gobernacion</t>
   </si>
   <si>
-    <t>asesores</t>
-  </si>
-  <si>
     <t>OPDAPAS</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>IMCUFIDEM</t>
   </si>
   <si>
-    <t>Transparencia</t>
-  </si>
-  <si>
     <t>Administracion</t>
   </si>
   <si>
@@ -125,25 +119,31 @@
     <t>Contraloria_Municipal</t>
   </si>
   <si>
-    <t>Comunicación_Social</t>
-  </si>
-  <si>
     <t>Gerencia_de_la_Ciudad</t>
   </si>
   <si>
     <t>Proteccion_Civil_y_Bomberos</t>
   </si>
   <si>
-    <t>Gobierno_digital</t>
-  </si>
-  <si>
-    <t>asuntos_religiosos</t>
-  </si>
-  <si>
     <t>Obras_Publicas</t>
   </si>
   <si>
-    <t>Defensora_Municipal_de_los_derechos_humanos</t>
+    <t>Asesores</t>
+  </si>
+  <si>
+    <t>Asuntos_Religosos</t>
+  </si>
+  <si>
+    <t>Comunicacion_Social</t>
+  </si>
+  <si>
+    <t>Defensoria_Municipal_de_los_Derechos_Humanos</t>
+  </si>
+  <si>
+    <t>Gobierno_Digital_y_Electronico</t>
+  </si>
+  <si>
+    <t>Transparencia_y_Gobierno_Abierto</t>
   </si>
 </sst>
 </file>
@@ -159,48 +159,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -215,17 +179,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EC664C-F74D-48DB-B806-F62A56262156}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,7 +534,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -589,7 +547,7 @@
       </c>
       <c r="E1">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -599,359 +557,359 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>116</v>
+        <v>30</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D28" si="0">SUM(B2:C2)</f>
-        <v>122</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F2">
         <f>(B2/E2)</f>
-        <v>0.22264875239923224</v>
+        <v>5.4545454545454543E-2</v>
       </c>
       <c r="G2">
         <f>(F2)*100</f>
-        <v>22.264875239923224</v>
+        <v>5.4545454545454541</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
+      <c r="A3" t="s">
+        <v>30</v>
       </c>
       <c r="B3">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F28" si="1">(B3/E3)</f>
-        <v>5.5662188099808059E-2</v>
+        <v>5.454545454545455E-3</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G28" si="2">(F3)*100</f>
-        <v>5.5662188099808061</v>
+        <v>0.54545454545454553</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>19</v>
+      <c r="A4" t="s">
+        <v>31</v>
       </c>
       <c r="B4">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>7.8694817658349334E-2</v>
+        <v>7.2727272727272727E-3</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>7.8694817658349336</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
+      <c r="A5" t="s">
+        <v>32</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>47</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>8.545454545454545E-2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>8.545454545454545</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>36</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E7">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>6.545454545454546E-2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>6.5454545454545459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.4545454545454545E-2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>1.4545454545454546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.4545454545454545E-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>1.4545454545454546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>2.5454545454545455E-2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>2.5454545454545454</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>1.6363636363636365E-2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>1.6363636363636365</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
         <v>5</v>
       </c>
-      <c r="E5">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>9.5969289827255271E-3</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="2"/>
-        <v>0.95969289827255266</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="E6">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>2.6871401151631478E-2</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
-        <v>2.6871401151631478</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>1.1516314779270634E-2</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>1.1516314779270633</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>48</v>
-      </c>
-      <c r="C8">
-        <v>16</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="E8">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>9.2130518234165071E-2</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>9.2130518234165066</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="E9">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>4.0307101727447218E-2</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>4.0307101727447217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
+      <c r="C13">
         <v>0</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>1.5355086372360844E-2</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
-        <v>1.5355086372360844</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11">
-        <v>23</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="E11">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>4.4145873320537425E-2</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
-        <v>4.4145873320537428</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12">
-        <v>26</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E12">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>4.9904030710172742E-2</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="2"/>
-        <v>4.9904030710172744</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E13">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>3.2629558541266791E-2</v>
+        <v>9.0909090909090905E-3</v>
       </c>
       <c r="G13">
         <f t="shared" si="2"/>
-        <v>3.262955854126679</v>
+        <v>0.90909090909090906</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>1.9193857965451054E-2</v>
+        <v>5.454545454545455E-3</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>1.9193857965451053</v>
+        <v>0.54545454545454553</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>17</v>
+      <c r="A15" t="s">
+        <v>8</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -965,74 +923,74 @@
       </c>
       <c r="E15">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>9.5969289827255271E-3</v>
+        <v>9.0909090909090905E-3</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>0.95969289827255266</v>
+        <v>0.90909090909090906</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>28</v>
+      <c r="A16" t="s">
+        <v>34</v>
       </c>
       <c r="B16">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="E16">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>6.71785028790787E-2</v>
+        <v>1.090909090909091E-2</v>
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>6.7178502879078703</v>
+        <v>1.0909090909090911</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
-        <v>10</v>
+      <c r="A17" t="s">
+        <v>24</v>
       </c>
       <c r="B17">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>4.0307101727447218E-2</v>
+        <v>3.090909090909091E-2</v>
       </c>
       <c r="G17">
         <f t="shared" si="2"/>
-        <v>4.0307101727447217</v>
+        <v>3.0909090909090908</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>12</v>
+      <c r="A18" t="s">
+        <v>11</v>
       </c>
       <c r="B18">
         <v>9</v>
@@ -1046,285 +1004,285 @@
       </c>
       <c r="E18">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>1.7274472168905951E-2</v>
+        <v>1.6363636363636365E-2</v>
       </c>
       <c r="G18">
         <f t="shared" si="2"/>
-        <v>1.727447216890595</v>
+        <v>1.6363636363636365</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>16</v>
+      <c r="A19" t="s">
+        <v>25</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E19">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>3.4548944337811902E-2</v>
+        <v>1.8181818181818181E-2</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>3.45489443378119</v>
+        <v>1.8181818181818181</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>4.7272727272727272E-2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>4.7272727272727275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B20">
-        <v>11</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="E20">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>2.1113243761996161E-2</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="2"/>
-        <v>2.1113243761996161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E21">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="1"/>
-        <v>5.7581573896353169E-3</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="2"/>
-        <v>0.57581573896353166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
       <c r="E22">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>9.5969289827255271E-3</v>
+        <v>1.4545454545454545E-2</v>
       </c>
       <c r="G22">
         <f t="shared" si="2"/>
-        <v>0.95969289827255266</v>
+        <v>1.4545454545454546</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E23">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F23">
         <f t="shared" si="1"/>
-        <v>5.7581573896353169E-3</v>
+        <v>0.04</v>
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>0.57581573896353166</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>31</v>
+      <c r="A24" t="s">
+        <v>14</v>
       </c>
       <c r="B24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E24">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>4.0307101727447218E-2</v>
+        <v>0.04</v>
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>4.0307101727447217</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="E25">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>1.1516314779270634E-2</v>
+        <v>9.8181818181818176E-2</v>
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>1.1516314779270633</v>
+        <v>9.8181818181818183</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E26">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>4.1818181818181817E-2</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>4.1818181818181817</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>120</v>
+      </c>
+      <c r="C27">
         <v>4</v>
       </c>
-      <c r="C26">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="E27">
+        <f>D29</f>
+        <v>550</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0.21818181818181817</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>21.818181818181817</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28">
         <v>0</v>
       </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E26">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="1"/>
-        <v>7.677543186180422E-3</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="2"/>
-        <v>0.76775431861804222</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27">
-        <v>8</v>
-      </c>
-      <c r="C27">
-        <v>5</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="E27">
-        <f>D29</f>
-        <v>521</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="1"/>
-        <v>1.5355086372360844E-2</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="2"/>
-        <v>1.5355086372360844</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28">
-        <v>8</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E28">
         <f>D29</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="F28">
         <f t="shared" si="1"/>
-        <v>1.5355086372360844E-2</v>
+        <v>1.090909090909091E-2</v>
       </c>
       <c r="G28">
         <f t="shared" si="2"/>
-        <v>1.5355086372360844</v>
+        <v>1.0909090909090911</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1333,18 +1291,18 @@
       </c>
       <c r="D29">
         <f>SUM(B2:B28)</f>
-        <v>521</v>
+        <v>550</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
       </c>
       <c r="F29">
         <f>SUM(F2:F28)</f>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <f>SUM(G2:G28)</f>
-        <v>99.999999999999972</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1353,7 +1311,7 @@
       </c>
       <c r="D30">
         <f>MEDIAN(D2:D27)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1378,6 +1336,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9d79ead9-ccf6-4ca1-bf50-acff66080910" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100747A2AC1B2A2EC4D9777D92AB3C1606A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="09a69fa5213838aa2509153927f32dac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9d79ead9-ccf6-4ca1-bf50-acff66080910" xmlns:ns4="570fb897-d274-4457-aa38-b13802a1744e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5f278dbff8306a56c26a3beb38da730" ns3:_="" ns4:_="">
     <xsd:import namespace="9d79ead9-ccf6-4ca1-bf50-acff66080910"/>
@@ -1604,24 +1579,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{534DA14E-2438-488D-BCE6-7785D8723E22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9d79ead9-ccf6-4ca1-bf50-acff66080910"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="570fb897-d274-4457-aa38-b13802a1744e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9d79ead9-ccf6-4ca1-bf50-acff66080910" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8087EB69-BA50-4370-90EF-9370E79F5015}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61C0F8AD-02DC-494A-81E4-AE7B61AFE288}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1638,29 +1621,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8087EB69-BA50-4370-90EF-9370E79F5015}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{534DA14E-2438-488D-BCE6-7785D8723E22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9d79ead9-ccf6-4ca1-bf50-acff66080910"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="570fb897-d274-4457-aa38-b13802a1744e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>